<commit_message>
Checklist en planning aangepast
</commit_message>
<xml_diff>
--- a/Docs/Plan_van_Aanpak/checklist pva .xlsx
+++ b/Docs/Plan_van_Aanpak/checklist pva .xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Project_P5\Docs\Plan_van_Aanpak\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t xml:space="preserve">A Algemeen, lay-out en taalgebruik van het plan van aanpak </t>
   </si>
@@ -289,15 +294,6 @@
   </si>
   <si>
     <t>Checklist Plan van Aanpak</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Controle door groep</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -306,11 +302,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -475,9 +471,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -527,7 +520,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -569,7 +562,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -601,9 +594,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,6 +629,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -810,1015 +805,995 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="36">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:4" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="B5" s="17"/>
-    </row>
-    <row r="6" spans="1:4" ht="45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="16"/>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="16.5" thickBot="1">
+    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="18.75">
+    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="18"/>
-    </row>
-    <row r="9" spans="1:4" ht="15.75">
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>1</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75">
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>1</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75">
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" ht="31.5">
+      <c r="B11" s="11"/>
+    </row>
+    <row r="12" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="12">
         <v>1</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="31.5">
+    <row r="13" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>92</v>
+      <c r="B13" s="12">
+        <v>1</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="12">
         <v>1</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75">
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="12">
         <v>1</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75">
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="12">
         <v>1</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75">
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" ht="18.75">
+      <c r="B17" s="13"/>
+    </row>
+    <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="14"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75">
+      <c r="B18" s="13"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="12">
         <v>1</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75">
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="12">
         <v>1</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="12">
         <v>1</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75">
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="12">
         <v>1</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75">
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="12">
         <v>1</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75">
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="12"/>
-    </row>
-    <row r="25" spans="1:4" ht="18.75">
+      <c r="B24" s="11"/>
+    </row>
+    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="12"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.75">
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="13"/>
+      <c r="B26" s="12">
+        <v>1</v>
+      </c>
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="31.5">
+    </row>
+    <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="13"/>
+      <c r="B27" s="12">
+        <v>1</v>
+      </c>
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75">
+    </row>
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="13"/>
+      <c r="B28" s="12">
+        <v>1</v>
+      </c>
       <c r="C28">
         <v>1</v>
       </c>
-      <c r="D28" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75">
+    </row>
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="13"/>
+      <c r="B29" s="12">
+        <v>1</v>
+      </c>
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="31.5">
+    </row>
+    <row r="30" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B30" s="12">
         <v>1</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="31.5">
+    <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="13"/>
+      <c r="B31" s="12">
+        <v>1</v>
+      </c>
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="47.25">
+    </row>
+    <row r="32" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="15">
-        <v>1</v>
-      </c>
-      <c r="C32" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="22.5">
+      <c r="B32" s="14"/>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="12"/>
-    </row>
-    <row r="34" spans="1:3" ht="45">
+      <c r="B33" s="11"/>
+    </row>
+    <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="12"/>
-    </row>
-    <row r="35" spans="1:3" ht="15.75">
-      <c r="A35" s="7"/>
-      <c r="B35" s="12"/>
-    </row>
-    <row r="36" spans="1:3" ht="18.75">
+      <c r="B34" s="11"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="11"/>
+    </row>
+    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="12"/>
-    </row>
-    <row r="37" spans="1:3" ht="31.5">
+      <c r="B36" s="11"/>
+    </row>
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="12">
         <v>1</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75">
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="13">
+      <c r="B38" s="12">
         <v>1</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75">
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="13">
+      <c r="B39" s="12">
         <v>1</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75">
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>91</v>
+      <c r="B40" s="18">
+        <v>1</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="20"/>
-    </row>
-    <row r="42" spans="1:3" ht="15.75">
+      <c r="B41" s="19"/>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="13">
+      <c r="B42" s="12">
         <v>1</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75">
+    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="13">
+      <c r="B43" s="12">
         <v>1</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75">
+    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="13">
+      <c r="B44" s="12">
         <v>1</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="18.75">
+    <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
-      <c r="B45" s="12"/>
-    </row>
-    <row r="46" spans="1:3" ht="18.75">
+      <c r="B45" s="11"/>
+    </row>
+    <row r="46" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="12"/>
-    </row>
-    <row r="47" spans="1:3" ht="15.75">
+      <c r="B46" s="11"/>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="13">
+      <c r="B47" s="12">
         <v>1</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75">
+    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B48" s="13">
+      <c r="B48" s="12">
         <v>1</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75">
+    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B49" s="13"/>
+      <c r="B49" s="12">
+        <v>1</v>
+      </c>
       <c r="C49">
         <v>1</v>
       </c>
-      <c r="D49" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="31.5">
+    </row>
+    <row r="50" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B50" s="13">
+      <c r="B50" s="12">
         <v>1</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75">
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B51" s="13"/>
+      <c r="B51" s="12">
+        <v>1</v>
+      </c>
       <c r="C51">
         <v>1</v>
       </c>
-      <c r="D51" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75">
+    </row>
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
-      <c r="B52" s="12"/>
-    </row>
-    <row r="53" spans="1:4" ht="18.75">
+      <c r="B52" s="11"/>
+    </row>
+    <row r="53" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B53" s="12"/>
-    </row>
-    <row r="54" spans="1:4" ht="15.75">
+      <c r="B53" s="11"/>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B54" s="13">
+      <c r="B54" s="12">
         <v>1</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75">
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B55" s="13">
+      <c r="B55" s="12">
         <v>1</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75">
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B56" s="13">
+      <c r="B56" s="12">
         <v>1</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75">
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B57" s="13">
+      <c r="B57" s="12">
         <v>1</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75">
+    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
-      <c r="B58" s="12"/>
-    </row>
-    <row r="59" spans="1:4" ht="18.75">
+      <c r="B58" s="11"/>
+    </row>
+    <row r="59" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B59" s="12"/>
-    </row>
-    <row r="60" spans="1:4" ht="31.5">
+      <c r="B59" s="11"/>
+    </row>
+    <row r="60" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B60" s="13">
+      <c r="B60" s="12">
         <v>1</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.75">
+    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B61" s="13">
+      <c r="B61" s="12">
         <v>1</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="31.5">
+    <row r="62" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B62" s="13">
+      <c r="B62" s="12">
         <v>1</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.75">
+    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
-      <c r="B63" s="12"/>
-    </row>
-    <row r="64" spans="1:4" ht="18.75">
+      <c r="B63" s="11"/>
+    </row>
+    <row r="64" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B64" s="12"/>
-    </row>
-    <row r="65" spans="1:4" ht="15.75">
+      <c r="B64" s="11"/>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B65" s="13">
+      <c r="B65" s="12">
         <v>1</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.75">
+    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B66" s="13">
+      <c r="B66" s="12">
         <v>1</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.75">
+    <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B67" s="13">
+      <c r="B67" s="12">
         <v>1</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.75">
+    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="13">
+      <c r="B68" s="12">
         <v>1</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75">
+    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
-      <c r="B69" s="12"/>
-    </row>
-    <row r="70" spans="1:4" ht="18.75">
+      <c r="B69" s="11"/>
+    </row>
+    <row r="70" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B70" s="12"/>
-    </row>
-    <row r="71" spans="1:4" ht="31.5">
+      <c r="B70" s="11"/>
+    </row>
+    <row r="71" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B71" s="13">
+      <c r="B71" s="12">
         <v>1</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="31.5">
+    <row r="72" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B72" s="13"/>
+      <c r="B72" s="12">
+        <v>1</v>
+      </c>
       <c r="C72">
         <v>1</v>
       </c>
-      <c r="D72" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="15.75">
+    </row>
+    <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B73" s="13">
+      <c r="B73" s="12">
         <v>1</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.75">
+    <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B74" s="13">
+      <c r="B74" s="12">
         <v>1</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.75">
+    <row r="75" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B75" s="13"/>
+      <c r="B75" s="12">
+        <v>1</v>
+      </c>
       <c r="C75">
         <v>1</v>
       </c>
-      <c r="D75" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="31.5">
+    </row>
+    <row r="76" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B76" s="13">
+      <c r="B76" s="12">
         <v>1</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.75">
+    <row r="77" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B77" s="13"/>
+      <c r="B77" s="12">
+        <v>1</v>
+      </c>
       <c r="C77">
         <v>1</v>
       </c>
-      <c r="D77" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="31.5">
+    </row>
+    <row r="78" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B78" s="13"/>
+      <c r="B78" s="12">
+        <v>1</v>
+      </c>
       <c r="C78">
         <v>1</v>
       </c>
-      <c r="D78" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="15.75">
+    </row>
+    <row r="79" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
-      <c r="B79" s="12"/>
-    </row>
-    <row r="80" spans="1:4" ht="18.75">
+      <c r="B79" s="11"/>
+    </row>
+    <row r="80" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B80" s="12"/>
-    </row>
-    <row r="81" spans="1:4" ht="15.75">
+      <c r="B80" s="11"/>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
-      <c r="B81" s="12"/>
-    </row>
-    <row r="82" spans="1:4" ht="18.75">
+      <c r="B81" s="11"/>
+    </row>
+    <row r="82" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B82" s="12"/>
-    </row>
-    <row r="83" spans="1:4" ht="15.75">
+      <c r="B82" s="11"/>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B83" s="13">
+      <c r="B83" s="12">
         <v>1</v>
       </c>
       <c r="C83">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.75">
+    <row r="84" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B84" s="13">
+      <c r="B84" s="12">
         <v>1</v>
       </c>
       <c r="C84">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="31.5">
+    <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B85" s="13"/>
+      <c r="B85" s="12">
+        <v>1</v>
+      </c>
       <c r="C85">
         <v>1</v>
       </c>
-      <c r="D85" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="15.75">
+    </row>
+    <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B86" s="13"/>
+      <c r="B86" s="12">
+        <v>1</v>
+      </c>
       <c r="C86">
         <v>1</v>
       </c>
-      <c r="D86" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="15.75">
+    </row>
+    <row r="87" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
-      <c r="B87" s="12"/>
-    </row>
-    <row r="88" spans="1:4" ht="18.75">
+      <c r="B87" s="11"/>
+    </row>
+    <row r="88" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B88" s="12"/>
-    </row>
-    <row r="89" spans="1:4" ht="31.5">
+      <c r="B88" s="11"/>
+    </row>
+    <row r="89" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B89" s="13">
+      <c r="B89" s="12">
         <v>1</v>
       </c>
       <c r="C89">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="31.5">
+    <row r="90" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B90" s="13">
+      <c r="B90" s="12">
         <v>1</v>
       </c>
       <c r="C90">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.75">
+    <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B91" s="13">
+      <c r="B91" s="12">
         <v>1</v>
       </c>
       <c r="C91">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.75">
+    <row r="92" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B92" s="13">
+      <c r="B92" s="12">
         <v>1</v>
       </c>
       <c r="C92">
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="31.5">
+    <row r="93" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B93" s="13"/>
+      <c r="B93" s="12">
+        <v>1</v>
+      </c>
       <c r="C93">
         <v>1</v>
       </c>
-      <c r="D93" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="31.5">
+    </row>
+    <row r="94" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B94" s="13"/>
+      <c r="B94" s="12">
+        <v>1</v>
+      </c>
       <c r="C94">
         <v>1</v>
       </c>
-      <c r="D94" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="15.75">
+    </row>
+    <row r="95" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B95" s="13">
+      <c r="B95" s="12">
         <v>1</v>
       </c>
       <c r="C95">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.75">
+    <row r="96" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
-      <c r="B96" s="12"/>
-    </row>
-    <row r="97" spans="1:4" ht="18.75">
+      <c r="B96" s="11"/>
+    </row>
+    <row r="97" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B97" s="12"/>
-    </row>
-    <row r="98" spans="1:4" ht="15.75">
+      <c r="B97" s="11"/>
+    </row>
+    <row r="98" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B98" s="13">
+      <c r="B98" s="12">
         <v>1</v>
       </c>
       <c r="C98">
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15.75">
+    <row r="99" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B99" s="13">
+      <c r="B99" s="12">
         <v>1</v>
       </c>
       <c r="C99">
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15.75">
+    <row r="100" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B100" s="13">
+      <c r="B100" s="12">
         <v>1</v>
       </c>
       <c r="C100">
         <v>1</v>
       </c>
-      <c r="D100" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="18.75">
+    </row>
+    <row r="101" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
-      <c r="B101" s="12"/>
-    </row>
-    <row r="102" spans="1:4" ht="18.75">
+      <c r="B101" s="11"/>
+    </row>
+    <row r="102" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B102" s="12"/>
-    </row>
-    <row r="103" spans="1:4" ht="15.75">
+      <c r="B102" s="11"/>
+    </row>
+    <row r="103" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B103" s="13">
+      <c r="B103" s="12">
         <v>1</v>
       </c>
       <c r="C103">
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15.75">
+    <row r="104" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B104" s="13">
+      <c r="B104" s="12">
         <v>1</v>
       </c>
       <c r="C104">
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15.75">
+    <row r="105" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B105" s="13">
+      <c r="B105" s="12">
         <v>1</v>
       </c>
       <c r="C105">
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15.75">
+    <row r="106" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B106" s="13">
+      <c r="B106" s="12">
         <v>1</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="31.5">
+    <row r="107" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B107" s="13">
+      <c r="B107" s="12">
         <v>1</v>
       </c>
       <c r="C107">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15.75">
+    <row r="108" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
-      <c r="B108" s="12"/>
-    </row>
-    <row r="109" spans="1:4" ht="18.75">
+      <c r="B108" s="11"/>
+    </row>
+    <row r="109" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B109" s="12"/>
-    </row>
-    <row r="110" spans="1:4" ht="16.5" thickBot="1">
+      <c r="B109" s="11"/>
+    </row>
+    <row r="110" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B110" s="16">
+      <c r="B110" s="15">
         <v>1</v>
       </c>
       <c r="C110">
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15.75">
-      <c r="A111" s="8" t="s">
+    <row r="111" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B111">
         <f t="shared" ref="B111:C111" si="0">SUM(B8:B110)</f>
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C111">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15.75">
-      <c r="A112" s="9" t="s">
+    <row r="112" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B112" s="10">
+      <c r="B112" s="9">
         <f>B111/$C111*10</f>
-        <v>7.5714285714285712</v>
+        <v>9.8571428571428577</v>
       </c>
     </row>
   </sheetData>
@@ -1829,7 +1804,7 @@
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FFFF7128"/>
         <color rgb="FFFFEF9C"/>
       </colorScale>
@@ -1841,33 +1816,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1920,24 +1898,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AFAB33E-1031-49BA-A588-1C5301A99807}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC4B3EB1-E67D-4B64-B435-42996348D439}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1958,9 +1927,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC4B3EB1-E67D-4B64-B435-42996348D439}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AFAB33E-1031-49BA-A588-1C5301A99807}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>